<commit_message>
New Submission Synced: 2026-02-04 18:51:28
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -692,7 +692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -707,25 +707,45 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Full Name</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Admission No</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>AI Score</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:51:28</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>YAYEEM IBRAHIM</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-04 18:56:30
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -692,7 +692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -739,13 +739,31 @@
           <t>YAYEEM IBRAHIM</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="C2" t="n">
+        <v>42</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:56:30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NAMBA MARCUS PULKA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-04 19:19:08
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -816,7 +816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -857,13 +857,31 @@
           <t>Zara Muhammad</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C2" t="n">
+        <v>38</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-04 19:19:08</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ANNABEL JOEL </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 12:24:25
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -780,14 +780,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Full Name</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Admission No</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>AI Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-07 12:24:25</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ahmed said Yusuf </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Number 14</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 17:58:31
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,14 +656,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Full Name</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Admission No</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>AI Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-07 17:58:31</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Name : Wabulari Zachariah </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 17:59:12
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -884,14 +884,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Full Name</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Admission No</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>AI Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-07 17:59:12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aisha modu sheriff </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 19:22:36
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -717,14 +717,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Full Name</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Admission No</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>AI Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-07 19:22:36</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SANI IBRAHIM SANI</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 19:35:18
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -717,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -758,13 +758,31 @@
           <t>SANI IBRAHIM SANI</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C2" t="n">
+        <v>19</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-07 19:35:18</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Arhyel Jacob wakawa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 19:37:39
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,13 +697,31 @@
           <t xml:space="preserve">Name : Wabulari Zachariah </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="C2" t="n">
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-07 19:37:39</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Muhammad dahiru idrisa </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 19:50:54
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -963,7 +963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,12 +1004,30 @@
           <t xml:space="preserve">Aisha modu sheriff </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="C2" t="n">
+        <v>15</v>
       </c>
       <c r="D2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-07 19:50:53</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moduye Khadija </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-07 20:00:19
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -814,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -879,13 +879,31 @@
           <t>NAMBA MARCUS PULKA</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="C3" t="n">
+        <v>39</v>
       </c>
       <c r="D3" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-07 20:00:19</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Muhammad Ali zarami</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 03:56:37
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,12 +715,30 @@
           <t xml:space="preserve">Muhammad dahiru idrisa </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="C3" t="n">
+        <v>14</v>
       </c>
       <c r="D3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-08 03:56:36</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SARAH MUSA BALAMI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 16:47:09
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -999,7 +999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1058,13 +1058,31 @@
           <t xml:space="preserve">Moduye Khadija </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C3" t="n">
+        <v>45</v>
       </c>
       <c r="D3" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-08 16:47:09</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ELISHA BITRUS DAUDA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 17:19:49
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -753,7 +753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,13 +812,31 @@
           <t>Arhyel Jacob wakawa</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="C3" t="n">
+        <v>22</v>
       </c>
       <c r="D3" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-08 17:19:49</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ummu Kalthum Muhammad Yahaya</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 17:46:18
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1017,7 +1017,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1094,13 +1094,31 @@
           <t>ELISHA BITRUS DAUDA</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C4" t="n">
+        <v>7</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-08 17:46:17</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ESTHER YAGA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 18:57:43
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,13 +733,31 @@
           <t>SARAH MUSA BALAMI</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C4" t="n">
+        <v>38</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-08 18:57:43</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Halima Sadiya Abubakar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:00:43
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -974,7 +974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1022,6 +1022,26 @@
       </c>
       <c r="D2" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:00:43</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Fatima Muhammed Gadaka</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:07:39
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -751,13 +751,31 @@
           <t>Halima Sadiya Abubakar</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="C5" t="n">
+        <v>25</v>
       </c>
       <c r="D5" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:07:39</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Amina Abubakar Adam</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:09:47
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1073,7 +1073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1168,13 +1168,31 @@
           <t>ESTHER YAGA</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="C5" t="n">
+        <v>32</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:09:47</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Iyudigal Fali</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:21:38
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,13 +769,31 @@
           <t>Amina Abubakar Adam</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="C6" t="n">
+        <v>47</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:21:37</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MUHAMMAD ABUBAKAR </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:27:05
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1091,7 +1091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,13 +1204,31 @@
           <t>Iyudigal Fali</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C6" t="n">
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:27:04</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FATIMA BUKAR WAZIRI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:38:02
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1091,7 +1091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,12 +1222,30 @@
           <t>FATIMA BUKAR WAZIRI</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="C7" t="n">
+        <v>33</v>
       </c>
       <c r="D7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:38:02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RAHAMA MOHAMMED YUSUF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:38:53
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1091,7 +1091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1240,13 +1240,31 @@
           <t>RAHAMA MOHAMMED YUSUF</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="C8" t="n">
+        <v>42</v>
       </c>
       <c r="D8" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:38:53</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GLORIA JOHN GADZAMA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:48:45
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -807,7 +807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -884,13 +884,31 @@
           <t>Ummu Kalthum Muhammad Yahaya</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="C4" t="n">
+        <v>43</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:48:45</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ibrahim Abubakar Shettima </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Number 3</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 19:58:11
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -807,7 +807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -909,6 +909,26 @@
       </c>
       <c r="D5" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-08 19:58:11</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Abdullahi Sugun Mai mele</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Number 35</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 20:20:44
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,13 +787,31 @@
           <t xml:space="preserve">MUHAMMAD ABUBAKAR </t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C7" t="n">
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-08 20:20:44</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rachel Michael</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 20:21:25
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1147,7 +1147,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1314,13 +1314,31 @@
           <t>GLORIA JOHN GADZAMA</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="C9" t="n">
+        <v>35</v>
       </c>
       <c r="D9" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-08 20:21:25</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shatu Musa Hassan </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 20:32:13
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1066,7 +1066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1134,6 +1134,26 @@
       </c>
       <c r="D3" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-08 20:32:13</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Yahya A Yahya</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 22:15:11
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1372,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1431,13 +1431,31 @@
           <t xml:space="preserve">ANNABEL JOEL </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="C3" t="n">
+        <v>28</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-08 22:15:10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Usman Muhammad Gubio</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 22:15:27
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1372,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1449,13 +1449,31 @@
           <t>Usman Muhammad Gubio</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="C4" t="n">
+        <v>5</v>
       </c>
       <c r="D4" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-08 22:15:27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Usman Muhammad Gubio</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 22:15:44
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1372,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1467,13 +1467,31 @@
           <t>Usman Muhammad Gubio</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="C5" t="n">
+        <v>5</v>
       </c>
       <c r="D5" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-08 22:15:44</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Usman Muhammad Gubio</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 22:15:58
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1372,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1485,13 +1485,31 @@
           <t>Usman Muhammad Gubio</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="C6" t="n">
+        <v>5</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-08 22:15:58</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Usman Muhammad Gubio</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-08 22:16:43
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1372,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1503,12 +1503,30 @@
           <t>Usman Muhammad Gubio</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-08 22:16:43</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Usman Muhammad Gubio</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 05:29:14
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -960,7 +960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1043,12 +1043,30 @@
           <t>Muhammad Ali zarami</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="C4" t="n">
+        <v>23</v>
       </c>
       <c r="D4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-09 05:29:14</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abubakar shettima mutawalli  </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 05:33:41
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1084,7 +1084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1172,6 +1172,26 @@
       </c>
       <c r="D4" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-09 05:33:41</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ibrahim Usman Umar </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 13:02:40
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1205,7 +1205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1390,13 +1390,31 @@
           <t xml:space="preserve">Shatu Musa Hassan </t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="C10" t="n">
+        <v>39</v>
       </c>
       <c r="D10" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-09 13:02:40</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Zainab Tijjani</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 13:31:48
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -825,7 +825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,6 +947,26 @@
       </c>
       <c r="D6" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-09 13:31:48</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>USMAN BABA SHEHU</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 17:14:02
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -980,7 +980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1081,13 +1081,31 @@
           <t xml:space="preserve">Abubakar shettima mutawalli  </t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C5" t="n">
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-09 17:14:02</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LAWAN SANI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 17:33:58
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -656,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -805,13 +805,31 @@
           <t>Rachel Michael</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="C8" t="n">
+        <v>34</v>
       </c>
       <c r="D8" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-09 17:33:58</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>JOHANNAH SALEM BOURMANDA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 17:43:43
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -843,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -984,6 +984,26 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-09 17:43:43</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ishaku Yusuf Dawha </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 17:45:32
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1281,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1484,13 +1484,31 @@
           <t>Zainab Tijjani</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C11" t="n">
+        <v>38</v>
       </c>
       <c r="D11" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-02-09 17:45:32</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Umar Fatima Ali</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 18:26:25
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1160,7 +1160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1267,6 +1267,26 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-09 18:26:25</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alamin hamza</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 19:24:17
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1160,7 +1160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1288,6 +1288,26 @@
       </c>
       <c r="D6" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-09 19:24:17</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mustapha Ali abbatar </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 20:40:31
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -843,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1005,6 +1005,26 @@
       </c>
       <c r="D8" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-09 20:40:31</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>musa peter</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-09 20:56:21
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1038,7 +1038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1157,13 +1157,31 @@
           <t>LAWAN SANI</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="C6" t="n">
+        <v>18</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-09 20:56:20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Hadiza Danjuma</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 14:21:14
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1038,7 +1038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1175,13 +1175,31 @@
           <t>Hadiza Danjuma</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="C7" t="n">
+        <v>31</v>
       </c>
       <c r="D7" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-10 14:21:14</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FATIMA ALHAJI GANA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 18:50:00
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -843,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,6 +1025,26 @@
       </c>
       <c r="D9" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-10 18:50:00</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Adam Muhammad Gudusu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 19:06:54
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1236,7 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1384,6 +1384,26 @@
       </c>
       <c r="D7" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-10 19:06:54</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mahmud Alhaji Hassan</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Number 5</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 19:13:10
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1236,7 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1404,6 +1404,26 @@
       </c>
       <c r="D8" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-10 19:13:10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aisha ahmed Talib </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Number 33</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 20:13:11
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1058,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1213,13 +1213,31 @@
           <t>FATIMA ALHAJI GANA</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C8" t="n">
+        <v>45</v>
       </c>
       <c r="D8" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-10 20:13:10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abatcha M Abatcha </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 20:15:45
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1254,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1442,6 +1442,26 @@
       </c>
       <c r="D9" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-10 20:15:44</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abubakar audu ali </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Number 7 </t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-10 22:35:32
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1254,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1462,6 +1462,26 @@
       </c>
       <c r="D10" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-10 22:35:31</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Audu Ali Abubakar </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-11 06:28:42
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1495,7 +1495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1716,12 +1716,30 @@
           <t>Umar Fatima Ali</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="C12" t="n">
+        <v>44</v>
       </c>
       <c r="D12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-02-11 06:28:42</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>HAUWA ALIYU MADUGU</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-12 07:39:40
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1254,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1482,6 +1482,26 @@
       </c>
       <c r="D11" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-02-12 07:39:40</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Abdullahi Tijjani Buji</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-12 19:51:17
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1254,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1502,6 +1502,26 @@
       </c>
       <c r="D12" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-02-12 19:51:17</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hauwa Hussaini maina</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-12 21:24:31
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -843,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,6 +1045,26 @@
       </c>
       <c r="D10" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-12 21:24:31</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nguru Ali </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Serial number 31</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Submission Synced: 2026-02-15 13:38:25
</commit_message>
<xml_diff>
--- a/Project_Results.xlsx
+++ b/Project_Results.xlsx
@@ -1274,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1542,6 +1542,26 @@
       </c>
       <c r="D13" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-15 13:38:25</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>muhammad musa usman</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>